<commit_message>
Test: Additional Prime Attribute tests
</commit_message>
<xml_diff>
--- a/DC20Models.nUnitTests/Unit Tests/Attribute/BlackBox_Attribute.xlsx
+++ b/DC20Models.nUnitTests/Unit Tests/Attribute/BlackBox_Attribute.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Blazor\DC20 Character Sheet\TestGeneration\Attribute\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Blazor\DC20 Character Sheet\DC20Models\DC20Models.nUnitTests\Unit Tests\Attribute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7834258-6AB4-417C-9E5B-91D57B7ACFD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD1CAAF-8C60-4E72-96FA-B4810E3E9DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{B6E2DC97-E5A5-4906-BB28-0603128A6FF0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B6E2DC97-E5A5-4906-BB28-0603128A6FF0}"/>
   </bookViews>
   <sheets>
     <sheet name="ValueTest" sheetId="1" r:id="rId1"/>
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B072AB2B-2B84-49ED-8A2B-DA516F62DDCB}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,33 +535,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="4"/>
+      <c r="I1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
@@ -574,9 +574,9 @@
       <c r="G2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -829,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86460E33-CEEB-4EE7-A91F-B5FF84DB84BE}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,32 +848,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="2" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
@@ -886,8 +886,8 @@
       <c r="G2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">

</xml_diff>